<commit_message>
Änderung der Concepz Classifiaction
</commit_message>
<xml_diff>
--- a/output/StructureDefinition-cde-age-at-diagnosis-of-essential-hypertension.xlsx
+++ b/output/StructureDefinition-cde-age-at-diagnosis-of-essential-hypertension.xlsx
@@ -60,7 +60,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2023-03-16T17:46:04+01:00</t>
+    <t>2023-03-17T18:03:12+01:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -4322,7 +4322,7 @@
         <v>92</v>
       </c>
       <c r="G16" t="s" s="2">
-        <v>92</v>
+        <v>81</v>
       </c>
       <c r="H16" t="s" s="2">
         <v>93</v>
@@ -5774,7 +5774,7 @@
         <v>92</v>
       </c>
       <c r="G28" t="s" s="2">
-        <v>92</v>
+        <v>81</v>
       </c>
       <c r="H28" t="s" s="2">
         <v>93</v>
@@ -7226,7 +7226,7 @@
         <v>92</v>
       </c>
       <c r="G40" t="s" s="2">
-        <v>92</v>
+        <v>81</v>
       </c>
       <c r="H40" t="s" s="2">
         <v>93</v>
@@ -8678,7 +8678,7 @@
         <v>92</v>
       </c>
       <c r="G52" t="s" s="2">
-        <v>92</v>
+        <v>81</v>
       </c>
       <c r="H52" t="s" s="2">
         <v>93</v>
@@ -10130,7 +10130,7 @@
         <v>92</v>
       </c>
       <c r="G64" t="s" s="2">
-        <v>92</v>
+        <v>81</v>
       </c>
       <c r="H64" t="s" s="2">
         <v>93</v>
@@ -11582,7 +11582,7 @@
         <v>92</v>
       </c>
       <c r="G76" t="s" s="2">
-        <v>92</v>
+        <v>81</v>
       </c>
       <c r="H76" t="s" s="2">
         <v>93</v>

</xml_diff>

<commit_message>
Update (#draft old CDEs)
</commit_message>
<xml_diff>
--- a/output/StructureDefinition-cde-age-at-diagnosis-of-essential-hypertension.xlsx
+++ b/output/StructureDefinition-cde-age-at-diagnosis-of-essential-hypertension.xlsx
@@ -51,7 +51,7 @@
     <t>Status</t>
   </si>
   <si>
-    <t>active</t>
+    <t>draft</t>
   </si>
   <si>
     <t>Experimental</t>
@@ -60,7 +60,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2023-03-30T02:04:17+02:00</t>
+    <t>2023-03-30T13:05:19+02:00</t>
   </si>
   <si>
     <t>Publisher</t>

</xml_diff>